<commit_message>
update figs with fontsize
</commit_message>
<xml_diff>
--- a/analyses_outputs/results.xlsx
+++ b/analyses_outputs/results.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -671,7 +671,7 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>results\Cohere-embed-multilingual-light-v3.0</t>
+          <t>Cohere-embed-multilingual-light-v3.0</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
@@ -756,7 +756,7 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>results\Cohere-embed-multilingual-v3.0</t>
+          <t>Cohere-embed-multilingual-v3.0</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">
@@ -841,7 +841,7 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>results\Geotrend\bert-base-10lang-cased</t>
+          <t>Geotrend/bert-base-10lang-cased</t>
         </is>
       </c>
       <c r="B6" s="2" t="n">
@@ -926,7 +926,7 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>results\Geotrend\bert-base-15lang-cased</t>
+          <t>Geotrend/bert-base-15lang-cased</t>
         </is>
       </c>
       <c r="B7" s="2" t="n">
@@ -1011,7 +1011,7 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>results\Geotrend\bert-base-25lang-cased</t>
+          <t>Geotrend/bert-base-25lang-cased</t>
         </is>
       </c>
       <c r="B8" s="2" t="n">
@@ -1096,7 +1096,7 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>results\Geotrend\distilbert-base-25lang-cased</t>
+          <t>Geotrend/distilbert-base-25lang-cased</t>
         </is>
       </c>
       <c r="B9" s="2" t="n">
@@ -1181,7 +1181,7 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>results\Geotrend\distilbert-base-en-fr-cased</t>
+          <t>Geotrend/distilbert-base-en-fr-cased</t>
         </is>
       </c>
       <c r="B10" s="2" t="n">
@@ -1266,7 +1266,7 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>results\Geotrend\distilbert-base-en-fr-es-pt-it-cased</t>
+          <t>Geotrend/distilbert-base-en-fr-es-pt-it-cased</t>
         </is>
       </c>
       <c r="B11" s="2" t="n">
@@ -1351,7 +1351,7 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>results\Geotrend\distilbert-base-fr-cased</t>
+          <t>Geotrend/distilbert-base-fr-cased</t>
         </is>
       </c>
       <c r="B12" s="2" t="n">
@@ -1436,7 +1436,7 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>results\Wissam42\sentence-croissant-llm-base</t>
+          <t>Wissam42/sentence-croissant-llm-base</t>
         </is>
       </c>
       <c r="B13" s="2" t="n">
@@ -1521,7 +1521,7 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>results\bert-base-multilingual-cased</t>
+          <t>bert-base-multilingual-cased</t>
         </is>
       </c>
       <c r="B14" s="2" t="n">
@@ -1606,7 +1606,7 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>results\bert-base-multilingual-uncased</t>
+          <t>bert-base-multilingual-uncased</t>
         </is>
       </c>
       <c r="B15" s="2" t="n">
@@ -1691,7 +1691,7 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>results\camembert\camembert-base</t>
+          <t>camembert/camembert-base</t>
         </is>
       </c>
       <c r="B16" s="2" t="n">
@@ -1776,7 +1776,7 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>results\camembert\camembert-large</t>
+          <t>camembert/camembert-large</t>
         </is>
       </c>
       <c r="B17" s="2" t="n">
@@ -1861,7 +1861,7 @@
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>results\dangvantuan\sentence-camembert-base</t>
+          <t>dangvantuan/sentence-camembert-base</t>
         </is>
       </c>
       <c r="B18" s="2" t="n">
@@ -1946,7 +1946,7 @@
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>results\dangvantuan\sentence-camembert-large</t>
+          <t>dangvantuan/sentence-camembert-large</t>
         </is>
       </c>
       <c r="B19" s="2" t="n">
@@ -2031,7 +2031,7 @@
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>results\distilbert-base-uncased</t>
+          <t>distilbert-base-uncased</t>
         </is>
       </c>
       <c r="B20" s="2" t="n">
@@ -2116,7 +2116,7 @@
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>results\flaubert\flaubert_base_cased</t>
+          <t>flaubert/flaubert_base_cased</t>
         </is>
       </c>
       <c r="B21" s="2" t="n">
@@ -2201,7 +2201,7 @@
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>results\flaubert\flaubert_base_uncased</t>
+          <t>flaubert/flaubert_base_uncased</t>
         </is>
       </c>
       <c r="B22" s="2" t="n">
@@ -2286,7 +2286,7 @@
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>results\flaubert\flaubert_large_cased</t>
+          <t>flaubert/flaubert_large_cased</t>
         </is>
       </c>
       <c r="B23" s="2" t="n">
@@ -2371,7 +2371,7 @@
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>results\intfloat\e5-mistral-7b-instruct</t>
+          <t>intfloat/e5-mistral-7b-instruct</t>
         </is>
       </c>
       <c r="B24" s="2" t="n">
@@ -2456,7 +2456,7 @@
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>results\intfloat\multilingual-e5-base</t>
+          <t>intfloat/multilingual-e5-base</t>
         </is>
       </c>
       <c r="B25" s="2" t="n">
@@ -2541,7 +2541,7 @@
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>results\intfloat\multilingual-e5-large</t>
+          <t>intfloat/multilingual-e5-large</t>
         </is>
       </c>
       <c r="B26" s="2" t="n">
@@ -2626,7 +2626,7 @@
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>results\intfloat\multilingual-e5-small</t>
+          <t>intfloat/multilingual-e5-small</t>
         </is>
       </c>
       <c r="B27" s="2" t="n">
@@ -2711,7 +2711,7 @@
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>results\izhx\udever-bloom-1b1</t>
+          <t>izhx/udever-bloom-1b1</t>
         </is>
       </c>
       <c r="B28" s="2" t="n">
@@ -2796,7 +2796,7 @@
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>results\izhx\udever-bloom-560m</t>
+          <t>izhx/udever-bloom-560m</t>
         </is>
       </c>
       <c r="B29" s="2" t="n">
@@ -2881,7 +2881,7 @@
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>results\laser2</t>
+          <t>laser2</t>
         </is>
       </c>
       <c r="B30" s="2" t="n">
@@ -2966,7 +2966,7 @@
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>results\sentence-transformers\LaBSE</t>
+          <t>sentence-transformers/LaBSE</t>
         </is>
       </c>
       <c r="B31" s="2" t="n">
@@ -3051,7 +3051,7 @@
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>results\sentence-transformers\all-MiniLM-L12-v2</t>
+          <t>sentence-transformers/all-MiniLM-L12-v2</t>
         </is>
       </c>
       <c r="B32" s="2" t="n">
@@ -3136,7 +3136,7 @@
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>results\sentence-transformers\all-MiniLM-L6-v2</t>
+          <t>sentence-transformers/all-MiniLM-L6-v2</t>
         </is>
       </c>
       <c r="B33" s="2" t="n">
@@ -3221,7 +3221,7 @@
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>results\sentence-transformers\distiluse-base-multilingual-cased-v2</t>
+          <t>sentence-transformers/distiluse-base-multilingual-cased-v2</t>
         </is>
       </c>
       <c r="B34" s="2" t="n">
@@ -3306,7 +3306,7 @@
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>results\sentence-transformers\multi-qa-MiniLM-L6-cos-v1</t>
+          <t>sentence-transformers/multi-qa-MiniLM-L6-cos-v1</t>
         </is>
       </c>
       <c r="B35" s="2" t="n">
@@ -3391,7 +3391,7 @@
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>results\sentence-transformers\paraphrase-multilingual-MiniLM-L12-v2</t>
+          <t>sentence-transformers/paraphrase-multilingual-MiniLM-L12-v2</t>
         </is>
       </c>
       <c r="B36" s="2" t="n">
@@ -3476,7 +3476,7 @@
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>results\sentence-transformers\paraphrase-multilingual-mpnet-base-v2</t>
+          <t>sentence-transformers/paraphrase-multilingual-mpnet-base-v2</t>
         </is>
       </c>
       <c r="B37" s="2" t="n">
@@ -3561,7 +3561,7 @@
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>results\sentence-transformers\sentence-t5-base</t>
+          <t>sentence-transformers/sentence-t5-base</t>
         </is>
       </c>
       <c r="B38" s="2" t="n">
@@ -3646,7 +3646,7 @@
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>results\sentence-transformers\sentence-t5-large</t>
+          <t>sentence-transformers/sentence-t5-large</t>
         </is>
       </c>
       <c r="B39" s="2" t="n">
@@ -3731,7 +3731,7 @@
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>results\sentence-transformers\sentence-t5-xl</t>
+          <t>sentence-transformers/sentence-t5-xl</t>
         </is>
       </c>
       <c r="B40" s="2" t="n">
@@ -3816,7 +3816,7 @@
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>results\sentence-transformers\sentence-t5-xxl</t>
+          <t>sentence-transformers/sentence-t5-xxl</t>
         </is>
       </c>
       <c r="B41" s="3" t="n">
@@ -3901,7 +3901,7 @@
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>results\shibing624\text2vec-base-multilingual</t>
+          <t>shibing624/text2vec-base-multilingual</t>
         </is>
       </c>
       <c r="B42" s="2" t="n">
@@ -3986,7 +3986,7 @@
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>results\text-embedding-ada-002</t>
+          <t>text-embedding-ada-002</t>
         </is>
       </c>
       <c r="B43" s="2" t="n">
@@ -4069,7 +4069,7 @@
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>results\voyage-2</t>
+          <t>voyage-2</t>
         </is>
       </c>
       <c r="B44" s="2" t="n">
@@ -4154,7 +4154,7 @@
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>results\voyage-code-2</t>
+          <t>voyage-code-2</t>
         </is>
       </c>
       <c r="B45" s="2" t="n">
@@ -4239,7 +4239,7 @@
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>results\vprelovac\universal-sentence-encoder-multilingual-3</t>
+          <t>vprelovac/universal-sentence-encoder-multilingual-3</t>
         </is>
       </c>
       <c r="B46" s="2" t="n">
@@ -4324,7 +4324,7 @@
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>results\vprelovac\universal-sentence-encoder-multilingual-large-3</t>
+          <t>vprelovac/universal-sentence-encoder-multilingual-large-3</t>
         </is>
       </c>
       <c r="B47" s="2" t="n">
@@ -4409,7 +4409,7 @@
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>results\xlm-roberta-base</t>
+          <t>xlm-roberta-base</t>
         </is>
       </c>
       <c r="B48" s="2" t="n">
@@ -4494,7 +4494,7 @@
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>results\xlm-roberta-large</t>
+          <t>xlm-roberta-large</t>
         </is>
       </c>
       <c r="B49" s="2" t="n">

</xml_diff>